<commit_message>
Corrigiendo la Base de Datos
</commit_message>
<xml_diff>
--- a/Datos/Data_Rev.xlsx
+++ b/Datos/Data_Rev.xlsx
@@ -115,7 +115,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="31">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,24 +203,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor rgb="FFCCCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor rgb="FFCCCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
@@ -268,12 +250,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor rgb="FFEFEFEF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor rgb="FFEFEFEF"/>
       </patternFill>
@@ -296,6 +272,54 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -309,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -334,18 +358,22 @@
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="M39" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -637,9 +665,9 @@
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" style="27" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" style="27" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="27" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="24" customWidth="1"/>
     <col min="7" max="7" width="6.42578125" style="11" customWidth="1"/>
     <col min="8" max="8" width="6.28515625" style="11" customWidth="1"/>
     <col min="9" max="9" width="6.42578125" style="14" customWidth="1"/>
@@ -659,16 +687,16 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="9" t="s">
@@ -727,16 +755,16 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="21">
         <v>100</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="22">
         <v>86</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="17">
         <v>29</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="19">
         <v>30</v>
       </c>
       <c r="H2" s="9">
@@ -774,10 +802,10 @@
         <f t="shared" si="2"/>
         <v>18.777777777777779</v>
       </c>
-      <c r="R2" s="1">
-        <v>0</v>
-      </c>
-      <c r="S2" s="34">
+      <c r="R2" s="32">
+        <v>1</v>
+      </c>
+      <c r="S2" s="30">
         <v>0</v>
       </c>
       <c r="T2" s="1">
@@ -794,25 +822,25 @@
       <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="34">
         <v>33</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="20">
         <v>71</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="23">
         <v>14</v>
       </c>
       <c r="G3" s="9">
         <v>50</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="19">
         <v>70</v>
       </c>
       <c r="I3" s="12">
         <v>1</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="33">
         <v>38</v>
       </c>
       <c r="K3" s="15">
@@ -847,8 +875,8 @@
       <c r="S3" s="1">
         <v>1</v>
       </c>
-      <c r="T3" s="1">
-        <v>1</v>
+      <c r="T3" s="30">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -861,16 +889,16 @@
       <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="21">
         <v>27</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="20">
         <v>30</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="23">
         <v>2</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="19">
         <v>30</v>
       </c>
       <c r="H4" s="9">
@@ -882,7 +910,7 @@
       <c r="J4" s="12">
         <v>10</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="37">
         <v>33</v>
       </c>
       <c r="L4" s="15">
@@ -928,22 +956,22 @@
       <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="26">
         <v>7</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="22">
         <v>11</v>
       </c>
       <c r="F5" s="17">
         <v>19</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="19">
         <v>20</v>
       </c>
       <c r="H5" s="9">
         <v>30</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="33">
         <v>5</v>
       </c>
       <c r="J5" s="12">
@@ -986,7 +1014,7 @@
       </c>
       <c r="U5">
         <f t="shared" ref="U5:W5" si="4">SUM(R2:R5)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="V5">
         <f t="shared" si="4"/>
@@ -994,7 +1022,7 @@
       </c>
       <c r="W5">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1007,13 +1035,13 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="21">
         <v>23</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="22">
         <v>54</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="25">
         <v>90</v>
       </c>
       <c r="G6" s="9">
@@ -1022,7 +1050,7 @@
       <c r="H6" s="9">
         <v>60</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="33">
         <v>85</v>
       </c>
       <c r="J6" s="12">
@@ -1054,7 +1082,7 @@
         <f t="shared" si="2"/>
         <v>-52.888888888888893</v>
       </c>
-      <c r="R6" s="33">
+      <c r="R6" s="29">
         <v>6</v>
       </c>
       <c r="S6" s="1">
@@ -1074,13 +1102,13 @@
       <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="26">
         <v>33</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="22">
         <v>26</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="25">
         <v>47</v>
       </c>
       <c r="G7" s="9">
@@ -1089,16 +1117,16 @@
       <c r="H7" s="9">
         <v>20</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="33">
         <v>45</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="33">
         <v>35</v>
       </c>
       <c r="K7" s="15">
         <v>59</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="37">
         <v>33</v>
       </c>
       <c r="M7">
@@ -1141,16 +1169,16 @@
       <c r="C8" s="1">
         <v>3</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="21">
         <v>14</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="20">
         <v>25</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="25">
         <v>30</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="19">
         <v>20</v>
       </c>
       <c r="H8" s="9">
@@ -1159,10 +1187,10 @@
       <c r="I8" s="12">
         <v>47</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="33">
         <v>26</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="37">
         <v>28</v>
       </c>
       <c r="L8" s="15">
@@ -1208,13 +1236,13 @@
       <c r="C9" s="1">
         <v>4</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="21">
         <v>7</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="22">
         <v>26</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="23">
         <v>9</v>
       </c>
       <c r="G9" s="9">
@@ -1287,13 +1315,13 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="21">
         <v>100</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="22">
         <v>30</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="23">
         <v>58</v>
       </c>
       <c r="G10" s="9">
@@ -1354,13 +1382,13 @@
       <c r="C11" s="1">
         <v>2</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="21">
         <v>40</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="38">
         <v>45</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="23">
         <v>52</v>
       </c>
       <c r="G11" s="9">
@@ -1378,7 +1406,7 @@
       <c r="K11" s="15">
         <v>18</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="37">
         <v>50</v>
       </c>
       <c r="M11">
@@ -1421,22 +1449,22 @@
       <c r="C12" s="1">
         <v>3</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="26">
         <v>60</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="20">
         <v>35</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="23">
         <v>35</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="19">
         <v>35</v>
       </c>
       <c r="H12" s="9">
         <v>27</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="33">
         <v>60</v>
       </c>
       <c r="J12" s="12">
@@ -1445,7 +1473,7 @@
       <c r="K12" s="15">
         <v>50</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="37">
         <v>30</v>
       </c>
       <c r="M12">
@@ -1488,22 +1516,22 @@
       <c r="C13" s="1">
         <v>4</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="26">
         <v>28</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="20">
         <v>25</v>
       </c>
       <c r="F13" s="17">
         <v>40</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="19">
         <v>28</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="19">
         <v>40</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="27">
         <v>30</v>
       </c>
       <c r="J13" s="12">
@@ -1567,13 +1595,13 @@
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="26">
         <v>25</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="22">
         <v>89</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="23">
         <v>82</v>
       </c>
       <c r="G14" s="9">
@@ -1585,13 +1613,13 @@
       <c r="I14" s="12">
         <v>9</v>
       </c>
-      <c r="J14" s="31">
+      <c r="J14" s="27">
         <v>21</v>
       </c>
       <c r="K14" s="15">
         <v>11</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="37">
         <v>26</v>
       </c>
       <c r="M14">
@@ -1634,10 +1662,10 @@
       <c r="C15" s="1">
         <v>2</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="21">
         <v>20</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="22">
         <v>19</v>
       </c>
       <c r="F15" s="17">
@@ -1646,7 +1674,7 @@
       <c r="G15" s="9">
         <v>43</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="19">
         <v>60</v>
       </c>
       <c r="I15" s="12">
@@ -1701,16 +1729,16 @@
       <c r="C16" s="1">
         <v>3</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="21">
         <v>45</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="22">
         <v>63</v>
       </c>
       <c r="F16" s="17">
         <v>17</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="19">
         <v>15</v>
       </c>
       <c r="H16" s="9">
@@ -1719,7 +1747,7 @@
       <c r="I16" s="12">
         <v>22</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J16" s="27">
         <v>17</v>
       </c>
       <c r="K16" s="15">
@@ -1768,31 +1796,31 @@
       <c r="C17" s="1">
         <v>4</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="26">
         <v>15</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="20">
         <v>27</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="23">
         <v>24</v>
       </c>
       <c r="G17" s="9">
         <v>56</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="19">
         <v>30</v>
       </c>
       <c r="I17" s="12">
         <v>32</v>
       </c>
-      <c r="J17" s="31">
+      <c r="J17" s="27">
         <v>12</v>
       </c>
       <c r="K17" s="15">
         <v>31</v>
       </c>
-      <c r="L17" s="15">
+      <c r="L17" s="37">
         <v>25</v>
       </c>
       <c r="M17">
@@ -1847,13 +1875,13 @@
       <c r="C18" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="21">
         <v>96</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="22">
         <v>32</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="23">
         <v>84</v>
       </c>
       <c r="G18" s="9">
@@ -1914,13 +1942,13 @@
       <c r="C19" s="1">
         <v>2</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="26">
         <v>25</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="22">
         <v>24</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="23">
         <v>63</v>
       </c>
       <c r="G19" s="9">
@@ -1929,7 +1957,7 @@
       <c r="H19" s="9">
         <v>37</v>
       </c>
-      <c r="I19" s="31">
+      <c r="I19" s="27">
         <v>30</v>
       </c>
       <c r="J19" s="12">
@@ -1981,13 +2009,13 @@
       <c r="C20" s="1">
         <v>3</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="21">
         <v>3</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="38">
         <v>35</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="23">
         <v>27</v>
       </c>
       <c r="G20" s="9">
@@ -2005,7 +2033,7 @@
       <c r="K20" s="15">
         <v>25</v>
       </c>
-      <c r="L20" s="15">
+      <c r="L20" s="37">
         <v>30</v>
       </c>
       <c r="M20">
@@ -2048,13 +2076,13 @@
       <c r="C21" s="1">
         <v>4</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="21">
         <v>81</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="22">
         <v>70</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="23">
         <v>17</v>
       </c>
       <c r="G21" s="9">
@@ -2127,13 +2155,13 @@
       <c r="C22" s="1">
         <v>1</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="21">
         <v>16</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="22">
         <v>60</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="23">
         <v>6</v>
       </c>
       <c r="G22" s="9">
@@ -2194,13 +2222,13 @@
       <c r="C23" s="1">
         <v>2</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="21">
         <v>32</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="22">
         <v>25</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="25">
         <v>23</v>
       </c>
       <c r="G23" s="9">
@@ -2209,7 +2237,7 @@
       <c r="H23" s="9">
         <v>40</v>
       </c>
-      <c r="I23" s="31">
+      <c r="I23" s="27">
         <v>18</v>
       </c>
       <c r="J23" s="12">
@@ -2261,10 +2289,10 @@
       <c r="C24" s="1">
         <v>3</v>
       </c>
-      <c r="D24" s="30">
+      <c r="D24" s="26">
         <v>12</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="22">
         <v>22</v>
       </c>
       <c r="F24" s="17">
@@ -2273,16 +2301,16 @@
       <c r="G24" s="9">
         <v>42</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="19">
         <v>19</v>
       </c>
-      <c r="I24" s="31">
+      <c r="I24" s="27">
         <v>16</v>
       </c>
       <c r="J24" s="12">
         <v>32</v>
       </c>
-      <c r="K24" s="15">
+      <c r="K24" s="37">
         <v>11</v>
       </c>
       <c r="L24" s="15">
@@ -2328,13 +2356,13 @@
       <c r="C25" s="1">
         <v>4</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="21">
         <v>55</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="38">
         <v>14</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="23">
         <v>6</v>
       </c>
       <c r="G25" s="9">
@@ -2349,7 +2377,7 @@
       <c r="J25" s="12">
         <v>20</v>
       </c>
-      <c r="K25" s="15">
+      <c r="K25" s="37">
         <v>18</v>
       </c>
       <c r="L25" s="15">
@@ -2407,13 +2435,13 @@
       <c r="C26" s="1">
         <v>1</v>
       </c>
-      <c r="D26" s="30">
+      <c r="D26" s="26">
         <v>12</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="20">
         <v>36</v>
       </c>
-      <c r="F26" s="28">
+      <c r="F26" s="25">
         <v>24</v>
       </c>
       <c r="G26" s="9">
@@ -2422,10 +2450,10 @@
       <c r="H26" s="9">
         <v>30</v>
       </c>
-      <c r="I26" s="31">
+      <c r="I26" s="27">
         <v>14</v>
       </c>
-      <c r="J26" s="31">
+      <c r="J26" s="27">
         <v>24</v>
       </c>
       <c r="K26" s="15">
@@ -2474,16 +2502,16 @@
       <c r="C27" s="1">
         <v>2</v>
       </c>
-      <c r="D27" s="30">
+      <c r="D27" s="26">
         <v>15</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="22">
         <v>72</v>
       </c>
       <c r="F27" s="17">
         <v>5</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="19">
         <v>10</v>
       </c>
       <c r="H27" s="9">
@@ -2492,7 +2520,7 @@
       <c r="I27" s="12">
         <v>32</v>
       </c>
-      <c r="J27" s="31">
+      <c r="J27" s="27">
         <v>16</v>
       </c>
       <c r="K27" s="15">
@@ -2541,25 +2569,25 @@
       <c r="C28" s="1">
         <v>3</v>
       </c>
-      <c r="D28" s="30">
+      <c r="D28" s="26">
         <v>24</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="20">
         <v>12</v>
       </c>
-      <c r="F28" s="26">
+      <c r="F28" s="23">
         <v>28</v>
       </c>
       <c r="G28" s="9">
         <v>40</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="19">
         <v>10</v>
       </c>
       <c r="I28" s="12">
         <v>9</v>
       </c>
-      <c r="J28" s="31">
+      <c r="J28" s="27">
         <v>22</v>
       </c>
       <c r="K28" s="15">
@@ -2608,19 +2636,19 @@
       <c r="C29" s="1">
         <v>4</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="21">
         <v>14</v>
       </c>
-      <c r="E29" s="23">
+      <c r="E29" s="20">
         <v>18</v>
       </c>
       <c r="F29" s="17">
         <v>20</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="19">
         <v>20</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="19">
         <v>16</v>
       </c>
       <c r="I29" s="12">
@@ -2629,7 +2657,7 @@
       <c r="J29" s="12">
         <v>32</v>
       </c>
-      <c r="K29" s="15">
+      <c r="K29" s="37">
         <v>18</v>
       </c>
       <c r="L29" s="15">
@@ -2687,10 +2715,10 @@
       <c r="C30" s="1">
         <v>1</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="21">
         <v>15</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="22">
         <v>35</v>
       </c>
       <c r="F30" s="17">
@@ -2699,7 +2727,7 @@
       <c r="G30" s="9">
         <v>6</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="19">
         <v>20</v>
       </c>
       <c r="I30" s="12">
@@ -2754,28 +2782,28 @@
       <c r="C31" s="1">
         <v>2</v>
       </c>
-      <c r="D31" s="30">
+      <c r="D31" s="26">
         <v>10</v>
       </c>
-      <c r="E31" s="23">
+      <c r="E31" s="20">
         <v>25</v>
       </c>
-      <c r="F31" s="26">
+      <c r="F31" s="23">
         <v>21</v>
       </c>
       <c r="G31" s="9">
         <v>15</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="19">
         <v>24</v>
       </c>
-      <c r="I31" s="31">
+      <c r="I31" s="27">
         <v>10</v>
       </c>
       <c r="J31" s="12">
         <v>30</v>
       </c>
-      <c r="K31" s="15">
+      <c r="K31" s="37">
         <v>28</v>
       </c>
       <c r="L31" s="15">
@@ -2821,31 +2849,31 @@
       <c r="C32" s="1">
         <v>3</v>
       </c>
-      <c r="D32" s="30">
+      <c r="D32" s="26">
         <v>25</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="20">
         <v>15</v>
       </c>
       <c r="F32" s="17">
         <v>13</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="19">
         <v>17</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="19">
         <v>12</v>
       </c>
-      <c r="I32" s="31">
+      <c r="I32" s="27">
         <v>20</v>
       </c>
-      <c r="J32" s="31">
+      <c r="J32" s="27">
         <v>10</v>
       </c>
-      <c r="K32" s="15">
+      <c r="K32" s="37">
         <v>15</v>
       </c>
-      <c r="L32" s="15">
+      <c r="L32" s="37">
         <v>28</v>
       </c>
       <c r="M32">
@@ -2888,31 +2916,31 @@
       <c r="C33" s="1">
         <v>4</v>
       </c>
-      <c r="D33" s="30">
+      <c r="D33" s="26">
         <v>13</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="22">
         <v>9</v>
       </c>
       <c r="F33" s="17">
         <v>8</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="19">
         <v>12</v>
       </c>
       <c r="H33" s="9">
         <v>17</v>
       </c>
-      <c r="I33" s="31">
+      <c r="I33" s="27">
         <v>17</v>
       </c>
-      <c r="J33" s="31">
+      <c r="J33" s="27">
         <v>10</v>
       </c>
       <c r="K33" s="15">
         <v>29</v>
       </c>
-      <c r="L33" s="15">
+      <c r="L33" s="37">
         <v>16</v>
       </c>
       <c r="M33">
@@ -2967,13 +2995,13 @@
       <c r="C34" s="1">
         <v>1</v>
       </c>
-      <c r="D34" s="24">
+      <c r="D34" s="21">
         <v>22</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="22">
         <v>60</v>
       </c>
-      <c r="F34" s="26">
+      <c r="F34" s="23">
         <v>76</v>
       </c>
       <c r="G34" s="9">
@@ -2988,7 +3016,7 @@
       <c r="J34" s="12">
         <v>63</v>
       </c>
-      <c r="K34" s="15">
+      <c r="K34" s="37">
         <v>25</v>
       </c>
       <c r="L34" s="15">
@@ -3034,16 +3062,16 @@
       <c r="C35" s="1">
         <v>2</v>
       </c>
-      <c r="D35" s="24">
+      <c r="D35" s="21">
         <v>17</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="22">
         <v>20</v>
       </c>
       <c r="F35" s="17">
         <v>48</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="19">
         <v>45</v>
       </c>
       <c r="H35" s="9">
@@ -3101,13 +3129,13 @@
       <c r="C36" s="1">
         <v>3</v>
       </c>
-      <c r="D36" s="24">
+      <c r="D36" s="21">
         <v>8</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E36" s="22">
         <v>10</v>
       </c>
-      <c r="F36" s="26">
+      <c r="F36" s="23">
         <v>33</v>
       </c>
       <c r="G36" s="9">
@@ -3125,7 +3153,7 @@
       <c r="K36" s="15">
         <v>30</v>
       </c>
-      <c r="L36" s="15">
+      <c r="L36" s="37">
         <v>15</v>
       </c>
       <c r="M36">
@@ -3168,19 +3196,19 @@
       <c r="C37" s="1">
         <v>4</v>
       </c>
-      <c r="D37" s="24">
+      <c r="D37" s="21">
         <v>3</v>
       </c>
-      <c r="E37" s="23">
+      <c r="E37" s="20">
         <v>8</v>
       </c>
       <c r="F37" s="17">
         <v>11</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="19">
         <v>10</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37" s="19">
         <v>12</v>
       </c>
       <c r="I37" s="12">
@@ -3189,7 +3217,7 @@
       <c r="J37" s="12">
         <v>19</v>
       </c>
-      <c r="K37" s="15">
+      <c r="K37" s="37">
         <v>7</v>
       </c>
       <c r="L37" s="15">
@@ -3247,16 +3275,16 @@
       <c r="C38" s="1">
         <v>1</v>
       </c>
-      <c r="D38" s="30">
+      <c r="D38" s="26">
         <v>22</v>
       </c>
-      <c r="E38" s="25">
+      <c r="E38" s="22">
         <v>8</v>
       </c>
       <c r="F38" s="17">
         <v>65</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="19">
         <v>65</v>
       </c>
       <c r="H38" s="9">
@@ -3265,7 +3293,7 @@
       <c r="I38" s="12">
         <v>15</v>
       </c>
-      <c r="J38" s="31">
+      <c r="J38" s="27">
         <v>23</v>
       </c>
       <c r="K38" s="15">
@@ -3314,16 +3342,16 @@
       <c r="C39" s="1">
         <v>2</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D39" s="21">
         <v>15</v>
       </c>
-      <c r="E39" s="23">
+      <c r="E39" s="20">
         <v>35</v>
       </c>
-      <c r="F39" s="26">
+      <c r="F39" s="23">
         <v>11</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="19">
         <v>33</v>
       </c>
       <c r="H39" s="9">
@@ -3335,7 +3363,7 @@
       <c r="J39" s="12">
         <v>66</v>
       </c>
-      <c r="K39" s="15">
+      <c r="K39" s="37">
         <v>30</v>
       </c>
       <c r="L39" s="15">
@@ -3381,31 +3409,31 @@
       <c r="C40" s="1">
         <v>3</v>
       </c>
-      <c r="D40" s="30">
+      <c r="D40" s="26">
         <v>7</v>
       </c>
-      <c r="E40" s="23">
+      <c r="E40" s="20">
         <v>15</v>
       </c>
       <c r="F40" s="17">
         <v>18</v>
       </c>
-      <c r="G40" s="9">
+      <c r="G40" s="19">
         <v>20</v>
       </c>
-      <c r="H40" s="9">
+      <c r="H40" s="19">
         <v>18</v>
       </c>
-      <c r="I40" s="31">
+      <c r="I40" s="27">
         <v>10</v>
       </c>
-      <c r="J40" s="31">
+      <c r="J40" s="27">
         <v>20</v>
       </c>
       <c r="K40" s="15">
         <v>20</v>
       </c>
-      <c r="L40" s="15">
+      <c r="L40" s="37">
         <v>15</v>
       </c>
       <c r="M40">
@@ -3448,22 +3476,22 @@
       <c r="C41" s="1">
         <v>4</v>
       </c>
-      <c r="D41" s="24">
+      <c r="D41" s="21">
         <v>3</v>
       </c>
-      <c r="E41" s="23">
+      <c r="E41" s="20">
         <v>5</v>
       </c>
       <c r="F41" s="17">
         <v>10</v>
       </c>
-      <c r="G41" s="9">
+      <c r="G41" s="19">
         <v>10</v>
       </c>
-      <c r="H41" s="9">
+      <c r="H41" s="19">
         <v>12</v>
       </c>
-      <c r="I41" s="31">
+      <c r="I41" s="27">
         <v>12</v>
       </c>
       <c r="J41" s="12">
@@ -3472,7 +3500,7 @@
       <c r="K41" s="15">
         <v>15</v>
       </c>
-      <c r="L41" s="15">
+      <c r="L41" s="37">
         <v>8</v>
       </c>
       <c r="M41">
@@ -3527,13 +3555,13 @@
       <c r="C42" s="1">
         <v>1</v>
       </c>
-      <c r="D42" s="24">
+      <c r="D42" s="21">
         <v>13</v>
       </c>
-      <c r="E42" s="25">
+      <c r="E42" s="22">
         <v>29</v>
       </c>
-      <c r="F42" s="26">
+      <c r="F42" s="23">
         <v>34</v>
       </c>
       <c r="G42" s="9">
@@ -3542,7 +3570,7 @@
       <c r="H42" s="9">
         <v>9</v>
       </c>
-      <c r="I42" s="31">
+      <c r="I42" s="27">
         <v>10</v>
       </c>
       <c r="J42" s="12">
@@ -3594,16 +3622,16 @@
       <c r="C43" s="1">
         <v>2</v>
       </c>
-      <c r="D43" s="24">
+      <c r="D43" s="21">
         <v>27</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E43" s="22">
         <v>33</v>
       </c>
       <c r="F43" s="17">
         <v>28</v>
       </c>
-      <c r="G43" s="9">
+      <c r="G43" s="19">
         <v>23</v>
       </c>
       <c r="H43" s="9">
@@ -3661,10 +3689,10 @@
       <c r="C44" s="1">
         <v>3</v>
       </c>
-      <c r="D44" s="24">
+      <c r="D44" s="21">
         <v>13</v>
       </c>
-      <c r="E44" s="25">
+      <c r="E44" s="22">
         <v>97</v>
       </c>
       <c r="F44" s="17">
@@ -3673,7 +3701,7 @@
       <c r="G44" s="9">
         <v>23</v>
       </c>
-      <c r="H44" s="9">
+      <c r="H44" s="19">
         <v>19</v>
       </c>
       <c r="I44" s="12">
@@ -3728,13 +3756,13 @@
       <c r="C45" s="1">
         <v>4</v>
       </c>
-      <c r="D45" s="24">
+      <c r="D45" s="21">
         <v>23</v>
       </c>
-      <c r="E45" s="25">
+      <c r="E45" s="22">
         <v>24</v>
       </c>
-      <c r="F45" s="26">
+      <c r="F45" s="23">
         <v>23</v>
       </c>
       <c r="G45" s="9">
@@ -3807,13 +3835,13 @@
       <c r="C46" s="1">
         <v>1</v>
       </c>
-      <c r="D46" s="24">
+      <c r="D46" s="39">
         <v>13</v>
       </c>
-      <c r="E46" s="25">
+      <c r="E46" s="22">
         <v>12</v>
       </c>
-      <c r="F46" s="26">
+      <c r="F46" s="23">
         <v>38</v>
       </c>
       <c r="G46" s="9">
@@ -3831,7 +3859,7 @@
       <c r="K46" s="15">
         <v>61</v>
       </c>
-      <c r="L46" s="15">
+      <c r="L46" s="37">
         <v>18</v>
       </c>
       <c r="M46">
@@ -3874,16 +3902,16 @@
       <c r="C47" s="1">
         <v>2</v>
       </c>
-      <c r="D47" s="24">
+      <c r="D47" s="21">
         <v>17</v>
       </c>
-      <c r="E47" s="23">
+      <c r="E47" s="20">
         <v>25</v>
       </c>
-      <c r="F47" s="28">
+      <c r="F47" s="25">
         <v>15</v>
       </c>
-      <c r="G47" s="9">
+      <c r="G47" s="19">
         <v>23</v>
       </c>
       <c r="H47" s="9">
@@ -3892,7 +3920,7 @@
       <c r="I47" s="12">
         <v>30</v>
       </c>
-      <c r="J47" s="31">
+      <c r="J47" s="27">
         <v>15</v>
       </c>
       <c r="K47" s="15">
@@ -3941,10 +3969,10 @@
       <c r="C48" s="1">
         <v>3</v>
       </c>
-      <c r="D48" s="30">
+      <c r="D48" s="26">
         <v>13</v>
       </c>
-      <c r="E48" s="25">
+      <c r="E48" s="22">
         <v>7</v>
       </c>
       <c r="F48" s="17">
@@ -3953,13 +3981,13 @@
       <c r="G48" s="9">
         <v>15</v>
       </c>
-      <c r="H48" s="9">
+      <c r="H48" s="19">
         <v>17</v>
       </c>
-      <c r="I48" s="31">
+      <c r="I48" s="27">
         <v>17</v>
       </c>
-      <c r="J48" s="31">
+      <c r="J48" s="27">
         <v>20</v>
       </c>
       <c r="K48" s="15">
@@ -4008,28 +4036,28 @@
       <c r="C49" s="1">
         <v>4</v>
       </c>
-      <c r="D49" s="24">
+      <c r="D49" s="39">
         <v>5</v>
       </c>
-      <c r="E49" s="23">
+      <c r="E49" s="20">
         <v>4</v>
       </c>
       <c r="F49" s="17">
         <v>12</v>
       </c>
-      <c r="G49" s="9">
+      <c r="G49" s="19">
         <v>5</v>
       </c>
-      <c r="H49" s="9">
+      <c r="H49" s="19">
         <v>17</v>
       </c>
       <c r="I49" s="12">
         <v>22</v>
       </c>
-      <c r="J49" s="31">
+      <c r="J49" s="27">
         <v>12</v>
       </c>
-      <c r="K49" s="15">
+      <c r="K49" s="37">
         <v>10</v>
       </c>
       <c r="L49" s="15">
@@ -4087,16 +4115,16 @@
       <c r="C50" s="1">
         <v>1</v>
       </c>
-      <c r="D50" s="24">
+      <c r="D50" s="21">
         <v>35</v>
       </c>
-      <c r="E50" s="23">
+      <c r="E50" s="20">
         <v>55</v>
       </c>
-      <c r="F50" s="26">
+      <c r="F50" s="23">
         <v>37</v>
       </c>
-      <c r="G50" s="9">
+      <c r="G50" s="19">
         <v>50</v>
       </c>
       <c r="H50" s="9">
@@ -4154,13 +4182,13 @@
       <c r="C51" s="1">
         <v>2</v>
       </c>
-      <c r="D51" s="30">
+      <c r="D51" s="26">
         <v>25</v>
       </c>
-      <c r="E51" s="25">
+      <c r="E51" s="22">
         <v>13</v>
       </c>
-      <c r="F51" s="26">
+      <c r="F51" s="23">
         <v>63</v>
       </c>
       <c r="G51" s="9">
@@ -4172,7 +4200,7 @@
       <c r="I51" s="12">
         <v>7</v>
       </c>
-      <c r="J51" s="31">
+      <c r="J51" s="27">
         <v>25</v>
       </c>
       <c r="K51" s="15">
@@ -4221,13 +4249,13 @@
       <c r="C52" s="1">
         <v>3</v>
       </c>
-      <c r="D52" s="30">
+      <c r="D52" s="26">
         <v>27</v>
       </c>
-      <c r="E52" s="25">
+      <c r="E52" s="22">
         <v>7</v>
       </c>
-      <c r="F52" s="26">
+      <c r="F52" s="23">
         <v>11</v>
       </c>
       <c r="G52" s="9">
@@ -4236,13 +4264,13 @@
       <c r="H52" s="9">
         <v>65</v>
       </c>
-      <c r="I52" s="31">
+      <c r="I52" s="27">
         <v>27</v>
       </c>
       <c r="J52" s="12">
         <v>62</v>
       </c>
-      <c r="K52" s="15">
+      <c r="K52" s="37">
         <v>25</v>
       </c>
       <c r="L52" s="15">
@@ -4288,16 +4316,16 @@
       <c r="C53" s="1">
         <v>4</v>
       </c>
-      <c r="D53" s="24">
+      <c r="D53" s="21">
         <v>15</v>
       </c>
-      <c r="E53" s="25">
+      <c r="E53" s="22">
         <v>68</v>
       </c>
       <c r="F53" s="17">
         <v>24</v>
       </c>
-      <c r="G53" s="9">
+      <c r="G53" s="19">
         <v>23</v>
       </c>
       <c r="H53" s="9">
@@ -4367,13 +4395,13 @@
       <c r="C54" s="1">
         <v>1</v>
       </c>
-      <c r="D54" s="24">
+      <c r="D54" s="39">
         <v>28</v>
       </c>
-      <c r="E54" s="25">
+      <c r="E54" s="22">
         <v>58</v>
       </c>
-      <c r="F54" s="26">
+      <c r="F54" s="23">
         <v>20</v>
       </c>
       <c r="G54" s="9">
@@ -4391,7 +4419,7 @@
       <c r="K54" s="15">
         <v>5</v>
       </c>
-      <c r="L54" s="15">
+      <c r="L54" s="37">
         <v>31</v>
       </c>
       <c r="M54">
@@ -4434,28 +4462,28 @@
       <c r="C55" s="1">
         <v>2</v>
       </c>
-      <c r="D55" s="30">
+      <c r="D55" s="26">
         <v>22</v>
       </c>
-      <c r="E55" s="25">
+      <c r="E55" s="22">
         <v>32</v>
       </c>
       <c r="F55" s="17">
         <v>35</v>
       </c>
-      <c r="G55" s="9">
+      <c r="G55" s="19">
         <v>40</v>
       </c>
       <c r="H55" s="9">
         <v>18</v>
       </c>
-      <c r="I55" s="31">
+      <c r="I55" s="27">
         <v>20</v>
       </c>
-      <c r="J55" s="31">
+      <c r="J55" s="27">
         <v>30</v>
       </c>
-      <c r="K55" s="15">
+      <c r="K55" s="37">
         <v>21</v>
       </c>
       <c r="L55" s="15">
@@ -4501,13 +4529,13 @@
       <c r="C56" s="1">
         <v>3</v>
       </c>
-      <c r="D56" s="30">
+      <c r="D56" s="26">
         <v>21</v>
       </c>
-      <c r="E56" s="25">
+      <c r="E56" s="22">
         <v>14</v>
       </c>
-      <c r="F56" s="28">
+      <c r="F56" s="25">
         <v>18</v>
       </c>
       <c r="G56" s="9">
@@ -4516,13 +4544,13 @@
       <c r="H56" s="9">
         <v>24</v>
       </c>
-      <c r="I56" s="31">
+      <c r="I56" s="27">
         <v>15</v>
       </c>
-      <c r="J56" s="31">
+      <c r="J56" s="27">
         <v>25</v>
       </c>
-      <c r="K56" s="15">
+      <c r="K56" s="37">
         <v>20</v>
       </c>
       <c r="L56" s="15">
@@ -4568,16 +4596,16 @@
       <c r="C57" s="1">
         <v>4</v>
       </c>
-      <c r="D57" s="24">
+      <c r="D57" s="21">
         <v>20</v>
       </c>
-      <c r="E57" s="23">
+      <c r="E57" s="20">
         <v>10</v>
       </c>
-      <c r="F57" s="26">
+      <c r="F57" s="23">
         <v>35</v>
       </c>
-      <c r="G57" s="9">
+      <c r="G57" s="19">
         <v>13</v>
       </c>
       <c r="H57" s="9">
@@ -4647,13 +4675,13 @@
       <c r="C58" s="1">
         <v>1</v>
       </c>
-      <c r="D58" s="25">
+      <c r="D58" s="22">
         <v>35</v>
       </c>
-      <c r="E58" s="24">
+      <c r="E58" s="21">
         <v>25</v>
       </c>
-      <c r="F58" s="26">
+      <c r="F58" s="23">
         <v>25</v>
       </c>
       <c r="G58" s="10">
@@ -4714,19 +4742,19 @@
       <c r="C59" s="1">
         <v>2</v>
       </c>
-      <c r="D59" s="25">
+      <c r="D59" s="38">
         <v>30</v>
       </c>
-      <c r="E59" s="22">
+      <c r="E59" s="19">
         <v>40</v>
       </c>
-      <c r="F59" s="26">
+      <c r="F59" s="23">
         <v>30</v>
       </c>
       <c r="G59" s="10">
         <v>20</v>
       </c>
-      <c r="H59" s="10">
+      <c r="H59" s="20">
         <v>40</v>
       </c>
       <c r="I59" s="13">
@@ -4735,7 +4763,7 @@
       <c r="J59" s="13">
         <v>10</v>
       </c>
-      <c r="K59" s="15">
+      <c r="K59" s="37">
         <v>30</v>
       </c>
       <c r="L59" s="15">
@@ -4781,25 +4809,25 @@
       <c r="C60" s="1">
         <v>3</v>
       </c>
-      <c r="D60" s="31">
+      <c r="D60" s="27">
         <v>25</v>
       </c>
-      <c r="E60" s="22">
+      <c r="E60" s="19">
         <v>33</v>
       </c>
-      <c r="F60" s="28">
+      <c r="F60" s="25">
         <v>35</v>
       </c>
       <c r="G60" s="10">
         <v>20</v>
       </c>
-      <c r="H60" s="10">
+      <c r="H60" s="20">
         <v>30</v>
       </c>
-      <c r="I60" s="30">
+      <c r="I60" s="26">
         <v>22</v>
       </c>
-      <c r="J60" s="30">
+      <c r="J60" s="26">
         <v>32</v>
       </c>
       <c r="K60" s="15">
@@ -4848,28 +4876,28 @@
       <c r="C61" s="1">
         <v>4</v>
       </c>
-      <c r="D61" s="31">
+      <c r="D61" s="27">
         <v>25</v>
       </c>
-      <c r="E61" s="24">
+      <c r="E61" s="39">
         <v>27</v>
       </c>
       <c r="F61" s="17">
         <v>30</v>
       </c>
-      <c r="G61" s="10">
+      <c r="G61" s="20">
         <v>30</v>
       </c>
       <c r="H61" s="10">
         <v>20</v>
       </c>
-      <c r="I61" s="30">
+      <c r="I61" s="26">
         <v>20</v>
       </c>
-      <c r="J61" s="30">
+      <c r="J61" s="26">
         <v>28</v>
       </c>
-      <c r="K61" s="15">
+      <c r="K61" s="37">
         <v>25</v>
       </c>
       <c r="L61" s="15">
@@ -4927,19 +4955,19 @@
       <c r="C62" s="1">
         <v>1</v>
       </c>
-      <c r="D62" s="24">
+      <c r="D62" s="21">
         <v>40</v>
       </c>
-      <c r="E62" s="23">
+      <c r="E62" s="20">
         <v>26</v>
       </c>
-      <c r="F62" s="26">
+      <c r="F62" s="23">
         <v>16</v>
       </c>
       <c r="G62" s="9">
         <v>50</v>
       </c>
-      <c r="H62" s="9">
+      <c r="H62" s="19">
         <v>30</v>
       </c>
       <c r="I62" s="12">
@@ -4948,7 +4976,7 @@
       <c r="J62" s="12">
         <v>32</v>
       </c>
-      <c r="K62" s="15">
+      <c r="K62" s="37">
         <v>23</v>
       </c>
       <c r="L62" s="15">
@@ -4994,10 +5022,10 @@
       <c r="C63" s="1">
         <v>2</v>
       </c>
-      <c r="D63" s="30">
+      <c r="D63" s="26">
         <v>20</v>
       </c>
-      <c r="E63" s="25">
+      <c r="E63" s="38">
         <v>35</v>
       </c>
       <c r="F63" s="17">
@@ -5006,19 +5034,19 @@
       <c r="G63" s="9">
         <v>15</v>
       </c>
-      <c r="H63" s="9">
+      <c r="H63" s="19">
         <v>25</v>
       </c>
       <c r="I63" s="12">
         <v>85</v>
       </c>
-      <c r="J63" s="31">
+      <c r="J63" s="27">
         <v>15</v>
       </c>
-      <c r="K63" s="15">
+      <c r="K63" s="37">
         <v>18</v>
       </c>
-      <c r="L63" s="15">
+      <c r="L63" s="37">
         <v>30</v>
       </c>
       <c r="M63">
@@ -5061,13 +5089,13 @@
       <c r="C64" s="1">
         <v>3</v>
       </c>
-      <c r="D64" s="24">
+      <c r="D64" s="39">
         <v>20</v>
       </c>
-      <c r="E64" s="25">
+      <c r="E64" s="22">
         <v>45</v>
       </c>
-      <c r="F64" s="26">
+      <c r="F64" s="23">
         <v>78</v>
       </c>
       <c r="G64" s="9">
@@ -5076,13 +5104,13 @@
       <c r="H64" s="9">
         <v>20</v>
       </c>
-      <c r="I64" s="31">
+      <c r="I64" s="27">
         <v>25</v>
       </c>
       <c r="J64" s="12">
         <v>65</v>
       </c>
-      <c r="K64" s="15">
+      <c r="K64" s="37">
         <v>20</v>
       </c>
       <c r="L64" s="15">
@@ -5128,13 +5156,13 @@
       <c r="C65" s="1">
         <v>4</v>
       </c>
-      <c r="D65" s="24">
+      <c r="D65" s="39">
         <v>28</v>
       </c>
-      <c r="E65" s="25">
+      <c r="E65" s="22">
         <v>14</v>
       </c>
-      <c r="F65" s="26">
+      <c r="F65" s="23">
         <v>51</v>
       </c>
       <c r="G65" s="9">
@@ -5149,7 +5177,7 @@
       <c r="J65" s="12">
         <v>85</v>
       </c>
-      <c r="K65" s="15">
+      <c r="K65" s="37">
         <v>27</v>
       </c>
       <c r="L65" s="15">
@@ -5207,13 +5235,13 @@
       <c r="C66" s="1">
         <v>1</v>
       </c>
-      <c r="D66" s="24">
+      <c r="D66" s="21">
         <v>45</v>
       </c>
-      <c r="E66" s="25">
+      <c r="E66" s="22">
         <v>95</v>
       </c>
-      <c r="F66" s="26">
+      <c r="F66" s="35">
         <v>6</v>
       </c>
       <c r="G66" s="9">
@@ -5225,7 +5253,7 @@
       <c r="I66" s="12">
         <v>25</v>
       </c>
-      <c r="J66" s="12">
+      <c r="J66" s="33">
         <v>4</v>
       </c>
       <c r="K66" s="15">
@@ -5274,13 +5302,13 @@
       <c r="C67" s="1">
         <v>2</v>
       </c>
-      <c r="D67" s="24">
+      <c r="D67" s="21">
         <v>55</v>
       </c>
-      <c r="E67" s="32">
+      <c r="E67" s="28">
         <v>23</v>
       </c>
-      <c r="F67" s="26">
+      <c r="F67" s="35">
         <v>28</v>
       </c>
       <c r="G67" s="9">
@@ -5292,7 +5320,7 @@
       <c r="I67" s="12">
         <v>15</v>
       </c>
-      <c r="J67" s="12">
+      <c r="J67" s="33">
         <v>30</v>
       </c>
       <c r="K67" s="15">
@@ -5341,10 +5369,10 @@
       <c r="C68" s="1">
         <v>3</v>
       </c>
-      <c r="D68" s="24">
+      <c r="D68" s="34">
         <v>30</v>
       </c>
-      <c r="E68" s="25">
+      <c r="E68" s="38">
         <v>40</v>
       </c>
       <c r="F68" s="17">
@@ -5353,19 +5381,19 @@
       <c r="G68" s="9">
         <v>25</v>
       </c>
-      <c r="H68" s="9">
+      <c r="H68" s="19">
         <v>35</v>
       </c>
       <c r="I68" s="12">
         <v>50</v>
       </c>
-      <c r="J68" s="12">
+      <c r="J68" s="33">
         <v>30</v>
       </c>
       <c r="K68" s="15">
         <v>20</v>
       </c>
-      <c r="L68" s="15">
+      <c r="L68" s="37">
         <v>40</v>
       </c>
       <c r="M68">
@@ -5408,13 +5436,13 @@
       <c r="C69" s="1">
         <v>4</v>
       </c>
-      <c r="D69" s="24">
+      <c r="D69" s="39">
         <v>25</v>
       </c>
-      <c r="E69" s="25">
+      <c r="E69" s="38">
         <v>35</v>
       </c>
-      <c r="F69" s="26">
+      <c r="F69" s="35">
         <v>34</v>
       </c>
       <c r="G69" s="9">
@@ -5426,13 +5454,13 @@
       <c r="I69" s="12">
         <v>45</v>
       </c>
-      <c r="J69" s="12">
+      <c r="J69" s="33">
         <v>35</v>
       </c>
-      <c r="K69" s="15">
+      <c r="K69" s="37">
         <v>35</v>
       </c>
-      <c r="L69" s="15">
+      <c r="L69" s="37">
         <v>25</v>
       </c>
       <c r="M69">
@@ -5487,10 +5515,10 @@
       <c r="C70" s="1">
         <v>1</v>
       </c>
-      <c r="D70" s="24">
+      <c r="D70" s="21">
         <v>55</v>
       </c>
-      <c r="E70" s="25">
+      <c r="E70" s="22">
         <v>60</v>
       </c>
       <c r="F70" s="17">
@@ -5499,13 +5527,13 @@
       <c r="G70" s="9">
         <v>80</v>
       </c>
-      <c r="H70" s="9">
+      <c r="H70" s="19">
         <v>15</v>
       </c>
       <c r="I70" s="12">
         <v>30</v>
       </c>
-      <c r="J70" s="12">
+      <c r="J70" s="33">
         <v>20</v>
       </c>
       <c r="K70" s="15">
@@ -5554,13 +5582,13 @@
       <c r="C71" s="1">
         <v>2</v>
       </c>
-      <c r="D71" s="24">
+      <c r="D71" s="39">
         <v>35</v>
       </c>
-      <c r="E71" s="25">
+      <c r="E71" s="38">
         <v>24</v>
       </c>
-      <c r="F71" s="26">
+      <c r="F71" s="35">
         <v>20</v>
       </c>
       <c r="G71" s="9">
@@ -5569,16 +5597,16 @@
       <c r="H71" s="9">
         <v>40</v>
       </c>
-      <c r="I71" s="12">
+      <c r="I71" s="33">
         <v>32</v>
       </c>
-      <c r="J71" s="12">
+      <c r="J71" s="33">
         <v>15</v>
       </c>
-      <c r="K71" s="15">
+      <c r="K71" s="37">
         <v>25</v>
       </c>
-      <c r="L71" s="15">
+      <c r="L71" s="37">
         <v>30</v>
       </c>
       <c r="M71">
@@ -5621,31 +5649,31 @@
       <c r="C72" s="1">
         <v>3</v>
       </c>
-      <c r="D72" s="24">
+      <c r="D72" s="34">
         <v>20</v>
       </c>
-      <c r="E72" s="23">
+      <c r="E72" s="20">
         <v>22</v>
       </c>
       <c r="F72" s="17">
         <v>19</v>
       </c>
-      <c r="G72" s="9">
+      <c r="G72" s="19">
         <v>25</v>
       </c>
-      <c r="H72" s="9">
+      <c r="H72" s="19">
         <v>20</v>
       </c>
-      <c r="I72" s="12">
+      <c r="I72" s="33">
         <v>24</v>
       </c>
       <c r="J72" s="12">
         <v>32</v>
       </c>
-      <c r="K72" s="15">
+      <c r="K72" s="37">
         <v>15</v>
       </c>
-      <c r="L72" s="15">
+      <c r="L72" s="37">
         <v>20</v>
       </c>
       <c r="M72">
@@ -5672,7 +5700,7 @@
         <v>2</v>
       </c>
       <c r="S72" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T72" s="1">
         <v>8</v>
@@ -5688,28 +5716,28 @@
       <c r="C73" s="1">
         <v>4</v>
       </c>
-      <c r="D73" s="24">
+      <c r="D73" s="34">
         <v>12</v>
       </c>
-      <c r="E73" s="23">
+      <c r="E73" s="20">
         <v>17</v>
       </c>
       <c r="F73" s="17">
         <v>16</v>
       </c>
-      <c r="G73" s="9">
+      <c r="G73" s="19">
         <v>15</v>
       </c>
-      <c r="H73" s="9">
+      <c r="H73" s="19">
         <v>17</v>
       </c>
-      <c r="I73" s="12">
+      <c r="I73" s="33">
         <v>18</v>
       </c>
-      <c r="J73" s="12">
+      <c r="J73" s="33">
         <v>13</v>
       </c>
-      <c r="K73" s="15">
+      <c r="K73" s="37">
         <v>18</v>
       </c>
       <c r="L73" s="15">
@@ -5750,7 +5778,7 @@
       </c>
       <c r="V73">
         <f t="shared" si="22"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W73">
         <f t="shared" si="22"/>
@@ -5767,16 +5795,16 @@
       <c r="C74" s="1">
         <v>1</v>
       </c>
-      <c r="D74" s="24">
+      <c r="D74" s="21">
         <v>90</v>
       </c>
-      <c r="E74" s="25">
+      <c r="E74" s="22">
         <v>15</v>
       </c>
       <c r="F74" s="17">
         <v>55</v>
       </c>
-      <c r="G74" s="9">
+      <c r="G74" s="19">
         <v>50</v>
       </c>
       <c r="H74" s="9">
@@ -5834,19 +5862,19 @@
       <c r="C75" s="1">
         <v>2</v>
       </c>
-      <c r="D75" s="24">
+      <c r="D75" s="21">
         <v>20</v>
       </c>
-      <c r="E75" s="23">
+      <c r="E75" s="20">
         <v>45</v>
       </c>
-      <c r="F75" s="26">
+      <c r="F75" s="23">
         <v>47</v>
       </c>
       <c r="G75" s="9">
         <v>30</v>
       </c>
-      <c r="H75" s="9">
+      <c r="H75" s="19">
         <v>40</v>
       </c>
       <c r="I75" s="12">
@@ -5901,13 +5929,13 @@
       <c r="C76" s="1">
         <v>3</v>
       </c>
-      <c r="D76" s="24">
+      <c r="D76" s="21">
         <v>40</v>
       </c>
-      <c r="E76" s="25">
+      <c r="E76" s="38">
         <v>35</v>
       </c>
-      <c r="F76" s="26">
+      <c r="F76" s="35">
         <v>35</v>
       </c>
       <c r="G76" s="9">
@@ -5919,13 +5947,13 @@
       <c r="I76" s="12">
         <v>55</v>
       </c>
-      <c r="J76" s="12">
+      <c r="J76" s="33">
         <v>30</v>
       </c>
-      <c r="K76" s="15">
+      <c r="K76" s="37">
         <v>30</v>
       </c>
-      <c r="L76" s="15">
+      <c r="L76" s="37">
         <v>45</v>
       </c>
       <c r="M76">
@@ -5968,10 +5996,10 @@
       <c r="C77" s="1">
         <v>4</v>
       </c>
-      <c r="D77" s="24">
+      <c r="D77" s="21">
         <v>30</v>
       </c>
-      <c r="E77" s="25">
+      <c r="E77" s="38">
         <v>45</v>
       </c>
       <c r="F77" s="17">
@@ -5980,19 +6008,19 @@
       <c r="G77" s="9">
         <v>20</v>
       </c>
-      <c r="H77" s="9">
+      <c r="H77" s="19">
         <v>40</v>
       </c>
       <c r="I77" s="12">
         <v>50</v>
       </c>
-      <c r="J77" s="12">
+      <c r="J77" s="33">
         <v>45</v>
       </c>
       <c r="K77" s="15">
         <v>40</v>
       </c>
-      <c r="L77" s="15">
+      <c r="L77" s="37">
         <v>45</v>
       </c>
       <c r="M77">
@@ -6047,22 +6075,22 @@
       <c r="C78" s="1">
         <v>1</v>
       </c>
-      <c r="D78" s="24">
+      <c r="D78" s="21">
         <v>35</v>
       </c>
-      <c r="E78" s="23">
+      <c r="E78" s="20">
         <v>15</v>
       </c>
-      <c r="F78" s="26">
+      <c r="F78" s="23">
         <v>32</v>
       </c>
       <c r="G78" s="9">
         <v>60</v>
       </c>
-      <c r="H78" s="22">
+      <c r="H78" s="19">
         <v>20</v>
       </c>
-      <c r="I78" s="12">
+      <c r="I78" s="33">
         <v>30</v>
       </c>
       <c r="J78" s="12">
@@ -6114,16 +6142,16 @@
       <c r="C79" s="1">
         <v>2</v>
       </c>
-      <c r="D79" s="24">
+      <c r="D79" s="34">
         <v>20</v>
       </c>
-      <c r="E79" s="25">
+      <c r="E79" s="22">
         <v>23</v>
       </c>
       <c r="F79" s="17">
         <v>28</v>
       </c>
-      <c r="G79" s="22">
+      <c r="G79" s="19">
         <v>30</v>
       </c>
       <c r="H79" s="9">
@@ -6132,10 +6160,10 @@
       <c r="I79" s="12">
         <v>55</v>
       </c>
-      <c r="J79" s="12">
+      <c r="J79" s="33">
         <v>22</v>
       </c>
-      <c r="K79" s="15">
+      <c r="K79" s="37">
         <v>16</v>
       </c>
       <c r="L79" s="15">
@@ -6181,25 +6209,25 @@
       <c r="C80" s="1">
         <v>3</v>
       </c>
-      <c r="D80" s="29">
+      <c r="D80" s="34">
         <v>25</v>
       </c>
-      <c r="E80" s="23">
+      <c r="E80" s="20">
         <v>18</v>
       </c>
-      <c r="F80" s="20">
+      <c r="F80" s="35">
         <v>43</v>
       </c>
-      <c r="G80" s="22">
+      <c r="G80" s="19">
         <v>20</v>
       </c>
       <c r="H80" s="9">
         <v>35</v>
       </c>
-      <c r="I80" s="21">
+      <c r="I80" s="33">
         <v>42</v>
       </c>
-      <c r="J80" s="21">
+      <c r="J80" s="33">
         <v>20</v>
       </c>
       <c r="K80" s="15">
@@ -6248,16 +6276,16 @@
       <c r="C81" s="1">
         <v>4</v>
       </c>
-      <c r="D81" s="30">
+      <c r="D81" s="34">
         <v>20</v>
       </c>
-      <c r="E81" s="19">
+      <c r="E81" s="18">
         <v>21</v>
       </c>
-      <c r="F81" s="28">
+      <c r="F81" s="36">
         <v>15</v>
       </c>
-      <c r="G81" s="22">
+      <c r="G81" s="19">
         <v>25</v>
       </c>
       <c r="H81" s="9">
@@ -6266,10 +6294,10 @@
       <c r="I81" s="12">
         <v>52</v>
       </c>
-      <c r="J81" s="21">
+      <c r="J81" s="33">
         <v>19</v>
       </c>
-      <c r="K81" s="18">
+      <c r="K81" s="37">
         <v>23</v>
       </c>
       <c r="L81" s="15">
@@ -6318,13 +6346,13 @@
       </c>
     </row>
     <row r="82" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D82" s="27" t="s">
+      <c r="D82" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E82" s="27" t="s">
+      <c r="E82" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F82" s="27" t="s">
+      <c r="F82" s="24" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>